<commit_message>
Committing the new tests for sprint 1 and 2 and the changes for the new  ROI page.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/LeadProcessWF_UsingSequence.xlsx
+++ b/src/main/resources/testdata/LeadProcessWF_UsingSequence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14745" windowHeight="4200"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12330" windowHeight="6285"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,47 +12,125 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+  <si>
+    <t>accessionNo</t>
+  </si>
+  <si>
+    <t>AF019145.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bharitkar S, Mendel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">search </t>
+  </si>
+  <si>
+    <t>AAA25689.1/AAA25689.1/</t>
+  </si>
+  <si>
+    <t>addSeq</t>
+  </si>
+  <si>
+    <t>abaxial stomatal frequency [en;XX;1]</t>
+  </si>
+  <si>
+    <t>Data#</t>
+  </si>
   <si>
     <t>Test_Description</t>
   </si>
   <si>
-    <t>Data#</t>
-  </si>
-  <si>
     <t>gene_type</t>
   </si>
   <si>
-    <t>nucleotide_seq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 421 atcgcgatgt caaagcgggg aatattttgc ttggtgctcg aggtgcagtc aagttgggag
-      481 actttggtgt atctgcatgt ctctttgatt caggtgatag gcaacgaaca aggaacacat
-      601 tcaaggctga tatttggtcg tttggtataa ctgggctaga gcttgctcat ggtcacgctc
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lead process workflow using nucleotide sequence</t>
-  </si>
-  <si>
     <t>Gene</t>
+  </si>
+  <si>
+    <t>Add Lead process workflow using Accession Number</t>
+  </si>
+  <si>
+    <t>newGFlink</t>
+  </si>
+  <si>
+    <t>mir1</t>
+  </si>
+  <si>
+    <t>rationale</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>observation</t>
+  </si>
+  <si>
+    <t>test observation</t>
+  </si>
+  <si>
+    <t>trait</t>
+  </si>
+  <si>
+    <t>AANV-2014</t>
+  </si>
+  <si>
+    <t>xrefAccessionNo</t>
+  </si>
+  <si>
+    <t>xrefSource</t>
+  </si>
+  <si>
+    <t>PlantGDB</t>
+  </si>
+  <si>
+    <t>suggestedProjectName</t>
+  </si>
+  <si>
+    <t>PI0000817:Soybean Rust Tolerance - NT</t>
+  </si>
+  <si>
+    <t>lead_source</t>
+  </si>
+  <si>
+    <t>Licensing</t>
+  </si>
+  <si>
+    <t>lead_type</t>
+  </si>
+  <si>
+    <t>gene</t>
+  </si>
+  <si>
+    <t>lead_function</t>
+  </si>
+  <si>
+    <t>test lead function</t>
+  </si>
+  <si>
+    <t>genie</t>
+  </si>
+  <si>
+    <t>source_lead_function_info</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -81,9 +159,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,63 +461,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="50.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" customWidth="1"/>
+    <col min="7" max="8" width="35.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.28515625" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" customWidth="1"/>
+    <col min="13" max="13" width="45" customWidth="1"/>
+    <col min="14" max="14" width="21.28515625" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" customWidth="1"/>
+    <col min="17" max="17" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30.5703125" customWidth="1"/>
+    <col min="19" max="19" width="26.85546875" customWidth="1"/>
+    <col min="20" max="20" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="s">
-        <v>4</v>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Committing the tests from Sprint 2 and for the database connection.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/LeadProcessWF_UsingSequence.xlsx
+++ b/src/main/resources/testdata/LeadProcessWF_UsingSequence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="12330" windowHeight="6285"/>
+    <workbookView xWindow="0" yWindow="1125" windowWidth="13650" windowHeight="5835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,21 +12,13 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
-    <t>accessionNo</t>
-  </si>
-  <si>
-    <t>AF019145.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bharitkar S, Mendel </t>
-  </si>
-  <si>
     <t xml:space="preserve">search </t>
   </si>
   <si>
@@ -51,9 +43,6 @@
     <t>Gene</t>
   </si>
   <si>
-    <t>Add Lead process workflow using Accession Number</t>
-  </si>
-  <si>
     <t>newGFlink</t>
   </si>
   <si>
@@ -115,6 +104,31 @@
   </si>
   <si>
     <t>source_lead_function_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTCGGATGATTCAAGCTCACGGGGACGAGCAGGAGCGCTCTCGACTTTTCTAGAGCCTCAGCGTCCTAGG
+ACTCACCTTTCCCTGATCCTGCACCGTCCCTCTCCTGGCCCCAGACTCTCCCTCCCACTGTTCACGAAGC
+CCAGGTGGGCCGTCGGCCGGGGAGCGGAGGGGGCGCGTGGGGTGCAGGCGGCGCCAAGGGCGCGTGCACC
+TGTGGGCGCGGGGCGCGAGGGCCCCTCCCGGCGCGAGCGGGCGCAGTTCCCCGGCGGCGCCGCTAGGGGT
+CTCTCTCGGGTGCCGAGCGGGGTGGGCCGGATCAGCTGACTCGCCTGGCTCTGAGCCCCGCCGCCGCGCT
+CGGGCTCCGTCAGTTTCCTCGGCAGCGGTAGGCGAGAGCACGCGGAGGAGCGTGCGCGGGGGCCCCGGGA
+GACGGCGGCGGTGGCGGCGCGGGCAGAGCAAGGACGCGGCGGATCCCACTCGCACAGCAGCGCACTCGGT
+GCCCCGCGCAGGGTCGCGATGCTGCCCGGTTTGGCACTGCTCCTGCTGGCCGCCTGGACGGCTCGGGCGC
+TGGAGGTGGGTGCCGCGCCTCGGAAGGCGGGGGGAGGCTGCACGGTGGGGACGCGATACCCCCCAAGACC
+TTAACCCAAGTCTTTAATGCAGAGAAGCCGGGGGTCCGTCAATGGGACCCCTCTCCTCTCCGCCCCCGCT
+TGCGGACGTCCAGCGCATCCCCGCTTTCGGCCCAGCCCTGCCCCAGGGAGTCGCGCTCCGGCCCGCTGAG
+AGGGAGCGGGCGAGGCGCTGGTCTCCCTGGTTCCGCGCCAGCCCGGGGCGAGAAGGGTAGGGGGCGACCC
+TGAGCCCAGACCCCGACTTAGTCCCTGCCTTGGAAGCGGGGGTCGGGGGAGGCGAGAGACATTCAGACAG
+</t>
+  </si>
+  <si>
+    <t>Add Lead process workflow using  Nucleotide sequence</t>
+  </si>
+  <si>
+    <t>addSequence</t>
+  </si>
+  <si>
+    <t>Butler KM</t>
   </si>
 </sst>
 </file>
@@ -157,9 +171,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,17 +480,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52" customWidth="1"/>
     <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" customWidth="1"/>
     <col min="6" max="6" width="35.5703125" customWidth="1"/>
     <col min="7" max="8" width="35.85546875" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -491,108 +508,108 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
       <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" t="s">
-        <v>29</v>
-      </c>
       <c r="Q1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="K2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" t="s">
-        <v>30</v>
-      </c>
       <c r="Q2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>